<commit_message>
add sth for every week
Signed-off-by: user2 <xtd412@qq.com>
</commit_message>
<xml_diff>
--- a/total_plan.xlsx
+++ b/total_plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -314,6 +314,18 @@
 3：EN reading
 4：聚传平台优化建议
 5：GERRIT搭建任务分配</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：聚传开发者拓展
+2：javaee day01
+3：英文阅读，
+4：中文阅读：网络形象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9:00-10:30.据传拓展
+10:30-11:30:javaday01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -884,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -990,7 +1002,7 @@
       <c r="M3" s="23"/>
       <c r="N3" s="24"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="144.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>42941</v>
       </c>
@@ -1010,11 +1022,13 @@
       <c r="M4" s="24"/>
       <c r="N4" s="25"/>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>42942</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -1031,9 +1045,13 @@
       <c r="A6" s="7">
         <v>42943</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="D6" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>

</xml_diff>